<commit_message>
changes in the TestBase class to make the running more easy. Added screenshot function and optimized reporting
</commit_message>
<xml_diff>
--- a/src/data/MIRO_Data.xlsx
+++ b/src/data/MIRO_Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE86F34-A3DE-47DF-953B-CDAF02363EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492C5B8C-C07A-4275-9B23-C16DAF8909DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MIRO_SIGNUP_TASK" sheetId="5" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Username</t>
   </si>
@@ -89,28 +89,31 @@
     <t>SignUpFailure</t>
   </si>
   <si>
-    <t>Test usern!_2321</t>
-  </si>
-  <si>
     <t>Username Special characters</t>
   </si>
   <si>
-    <t>Test usernameßüöä</t>
-  </si>
-  <si>
     <t>German special characters with user name and password</t>
   </si>
   <si>
-    <t>ProperEmail1111@gmail.com</t>
-  </si>
-  <si>
-    <t>Proper1112331@gmail.com</t>
-  </si>
-  <si>
-    <t>ProperProperEmaila1222!2_2@gmail.com</t>
-  </si>
-  <si>
     <t>EmailEmail191@gmail.com</t>
+  </si>
+  <si>
+    <t>Testdf usern!_2321</t>
+  </si>
+  <si>
+    <t>Proper11127451@gmail.com</t>
+  </si>
+  <si>
+    <t>Test12bcv usernamer</t>
+  </si>
+  <si>
+    <t>PrbfjaEqwkil1111@gmail.com</t>
+  </si>
+  <si>
+    <t>Pr2operEmaila1222!2_2@gmail.com</t>
+  </si>
+  <si>
+    <t>Test usernameßüöäe</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,10 +636,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
@@ -655,16 +658,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="3"/>
@@ -677,16 +680,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="3"/>
@@ -702,7 +705,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>4</v>

</xml_diff>